<commit_message>
Adding more dates to special dates
</commit_message>
<xml_diff>
--- a/Descriptiva y depuracion/dias_espe.xlsx
+++ b/Descriptiva y depuracion/dias_espe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JF_Mra\Documents\GitHub\accidentes_medellin\Descriptiva y depuracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidChaverraMunera\Desktop\github\Proyecto_1_TAE\accidentes_medellin\Descriptiva y depuracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D197FA5-12C7-45AE-82B8-1D7EAEB0DCDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEB22F5-4441-41DC-A8D6-56AA425E74E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{50B1CA56-B962-4D3E-BD9B-8EB443714974}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" xr2:uid="{50B1CA56-B962-4D3E-BD9B-8EB443714974}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,13 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A604231-3C0A-4FEF-96E8-A4BDCFC342A8}">
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -428,7 +430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,7 +441,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>13</v>
       </c>
@@ -450,7 +452,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>24</v>
       </c>
@@ -461,7 +463,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -472,7 +474,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>17</v>
       </c>
@@ -483,7 +485,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>18</v>
       </c>
@@ -494,7 +496,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -505,7 +507,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -516,7 +518,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>11</v>
       </c>
@@ -527,7 +529,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -538,7 +540,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>23</v>
       </c>
@@ -549,7 +551,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>30</v>
       </c>
@@ -560,7 +562,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
@@ -571,7 +573,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -582,7 +584,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>18</v>
       </c>
@@ -593,7 +595,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -604,7 +606,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -615,7 +617,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -626,7 +628,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8</v>
       </c>
@@ -637,7 +639,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -648,7 +650,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>31</v>
       </c>
@@ -659,7 +661,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -670,7 +672,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -681,7 +683,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -692,7 +694,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>29</v>
       </c>
@@ -703,7 +705,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -714,7 +716,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -725,7 +727,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -736,7 +738,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -747,7 +749,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>
@@ -758,7 +760,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>18</v>
       </c>
@@ -769,7 +771,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
@@ -780,7 +782,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>16</v>
       </c>
@@ -791,7 +793,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>29</v>
       </c>
@@ -802,7 +804,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -813,7 +815,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>7</v>
       </c>
@@ -824,7 +826,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>17</v>
       </c>
@@ -835,7 +837,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -846,7 +848,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
@@ -857,7 +859,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>16</v>
       </c>
@@ -868,7 +870,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>8</v>
       </c>
@@ -879,7 +881,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>25</v>
       </c>
@@ -890,7 +892,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>31</v>
       </c>
@@ -901,7 +903,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -912,7 +914,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>11</v>
       </c>
@@ -923,7 +925,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>20</v>
       </c>
@@ -934,7 +936,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>21</v>
       </c>
@@ -945,7 +947,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>24</v>
       </c>
@@ -956,7 +958,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>25</v>
       </c>
@@ -967,7 +969,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>27</v>
       </c>
@@ -978,7 +980,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
@@ -989,7 +991,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>8</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>9</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>30</v>
       </c>
@@ -1022,7 +1024,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>20</v>
       </c>
@@ -1055,7 +1057,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>7</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>17</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>17</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>7</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>8</v>
       </c>
@@ -1132,7 +1134,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>25</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>31</v>
       </c>
@@ -1154,7 +1156,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>9</v>
       </c>
@@ -1176,7 +1178,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20</v>
       </c>
@@ -1187,7 +1189,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>9</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>13</v>
       </c>
@@ -1209,7 +1211,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>14</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>16</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1242,7 +1244,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>14</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>29</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>19</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>26</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>3</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>7</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>21</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>16</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>6</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>13</v>
       </c>
@@ -1363,7 +1365,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>8</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>25</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>31</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>8</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>19</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>25</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>29</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>30</v>
       </c>
@@ -1462,7 +1464,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>13</v>
       </c>
@@ -1495,7 +1497,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>14</v>
       </c>
@@ -1506,7 +1508,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
@@ -1517,7 +1519,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>11</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>20</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>7</v>
       </c>
@@ -1561,7 +1563,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>20</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>15</v>
       </c>
@@ -1583,7 +1585,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5</v>
       </c>
@@ -1594,7 +1596,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>12</v>
       </c>
@@ -1605,7 +1607,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>8</v>
       </c>
@@ -1616,7 +1618,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>25</v>
       </c>
@@ -1627,7 +1629,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>31</v>
       </c>
@@ -1638,7 +1640,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>22</v>
       </c>
@@ -1649,7 +1651,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>22</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>21</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>24</v>
       </c>
@@ -1680,6 +1682,451 @@
       </c>
       <c r="C115" s="3">
         <v>2018</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="3">
+        <v>1</v>
+      </c>
+      <c r="B116" s="3">
+        <v>1</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
+        <v>7</v>
+      </c>
+      <c r="B117" s="3">
+        <v>1</v>
+      </c>
+      <c r="C117" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="3">
+        <v>25</v>
+      </c>
+      <c r="B118" s="3">
+        <v>3</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="3">
+        <v>14</v>
+      </c>
+      <c r="B119" s="3">
+        <v>4</v>
+      </c>
+      <c r="C119" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="3">
+        <v>18</v>
+      </c>
+      <c r="B120" s="3">
+        <v>4</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="3">
+        <v>19</v>
+      </c>
+      <c r="B121" s="3">
+        <v>4</v>
+      </c>
+      <c r="C121" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="3">
+        <v>21</v>
+      </c>
+      <c r="B122" s="3">
+        <v>4</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
+        <v>1</v>
+      </c>
+      <c r="B123" s="3">
+        <v>5</v>
+      </c>
+      <c r="C123" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="3">
+        <v>12</v>
+      </c>
+      <c r="B124" s="3">
+        <v>5</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>3</v>
+      </c>
+      <c r="B125" s="3">
+        <v>6</v>
+      </c>
+      <c r="C125" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>16</v>
+      </c>
+      <c r="B126" s="3">
+        <v>6</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="3">
+        <v>24</v>
+      </c>
+      <c r="B127" s="3">
+        <v>6</v>
+      </c>
+      <c r="C127" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="3">
+        <v>1</v>
+      </c>
+      <c r="B128" s="3">
+        <v>7</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="3">
+        <v>20</v>
+      </c>
+      <c r="B129" s="3">
+        <v>7</v>
+      </c>
+      <c r="C129" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="3">
+        <v>7</v>
+      </c>
+      <c r="B130" s="3">
+        <v>8</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="3">
+        <v>19</v>
+      </c>
+      <c r="B131" s="3">
+        <v>8</v>
+      </c>
+      <c r="C131" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="3">
+        <v>14</v>
+      </c>
+      <c r="B132" s="3">
+        <v>10</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="3">
+        <v>31</v>
+      </c>
+      <c r="B133" s="3">
+        <v>10</v>
+      </c>
+      <c r="C133" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="3">
+        <v>4</v>
+      </c>
+      <c r="B134" s="3">
+        <v>11</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="3">
+        <v>11</v>
+      </c>
+      <c r="B135" s="3">
+        <v>11</v>
+      </c>
+      <c r="C135" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="3">
+        <v>7</v>
+      </c>
+      <c r="B136" s="3">
+        <v>12</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="3">
+        <v>8</v>
+      </c>
+      <c r="B137" s="3">
+        <v>12</v>
+      </c>
+      <c r="C137" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="3">
+        <v>25</v>
+      </c>
+      <c r="B138" s="3">
+        <v>12</v>
+      </c>
+      <c r="C138" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="3">
+        <v>1</v>
+      </c>
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="3">
+        <v>6</v>
+      </c>
+      <c r="B140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="3">
+        <v>23</v>
+      </c>
+      <c r="B141" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="3">
+        <v>5</v>
+      </c>
+      <c r="B142" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="3">
+        <v>9</v>
+      </c>
+      <c r="B143" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="3">
+        <v>10</v>
+      </c>
+      <c r="B144" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="3">
+        <v>12</v>
+      </c>
+      <c r="B145" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="3">
+        <v>1</v>
+      </c>
+      <c r="B146" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="3">
+        <v>10</v>
+      </c>
+      <c r="B147" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="3">
+        <v>25</v>
+      </c>
+      <c r="B148" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="3">
+        <v>15</v>
+      </c>
+      <c r="B149" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="3">
+        <v>21</v>
+      </c>
+      <c r="B150" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="3">
+        <v>22</v>
+      </c>
+      <c r="B151" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="3">
+        <v>29</v>
+      </c>
+      <c r="B152" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="3">
+        <v>20</v>
+      </c>
+      <c r="B153" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="3">
+        <v>7</v>
+      </c>
+      <c r="B154" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="3">
+        <v>17</v>
+      </c>
+      <c r="B155" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="3">
+        <v>12</v>
+      </c>
+      <c r="B156" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="3">
+        <v>31</v>
+      </c>
+      <c r="B157" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="3">
+        <v>2</v>
+      </c>
+      <c r="B158" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="3">
+        <v>16</v>
+      </c>
+      <c r="B159" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="3">
+        <v>7</v>
+      </c>
+      <c r="B160" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="3">
+        <v>8</v>
+      </c>
+      <c r="B161" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="3">
+        <v>25</v>
+      </c>
+      <c r="B162" s="3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>